<commit_message>
Improve layout and functionality with enhanced header display and route management
</commit_message>
<xml_diff>
--- a/A Week Deliveries 2025.xlsx
+++ b/A Week Deliveries 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e053b881a0417d76/Projects/biruks-egg-deliveries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{5A90093B-DA4F-3A4F-939A-B6EFE387899A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36645971-A6A1-4549-AC64-AE99A094ABC3}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{5A90093B-DA4F-3A4F-939A-B6EFE387899A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EE6BC10-E37B-1D40-B50A-3D830B5C8E12}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="8580" windowWidth="28800" windowHeight="16280" xr2:uid="{C13AF774-5AE5-3F44-8572-B15CCF6D1D7C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="239">
   <si>
     <t>Name</t>
   </si>
@@ -565,9 +565,6 @@
     <t>1000 N. College</t>
   </si>
   <si>
-    <t>#news</t>
-  </si>
-  <si>
     <t>Canton newsletters (some are each week deliveries, so need to be accounted for)</t>
   </si>
   <si>
@@ -743,6 +740,21 @@
   </si>
   <si>
     <t>316 S. Main</t>
+  </si>
+  <si>
+    <t>Week A</t>
+  </si>
+  <si>
+    <t>CUST001</t>
+  </si>
+  <si>
+    <t>CUST002</t>
+  </si>
+  <si>
+    <t>CUST003</t>
+  </si>
+  <si>
+    <t>Newsletter</t>
   </si>
 </sst>
 </file>
@@ -1128,27 +1140,31 @@
   <dimension ref="A1:K95"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="41.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" style="1" customWidth="1"/>
-    <col min="10" max="10" width="74.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="73.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1157,39 +1173,45 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>37</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>175</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
@@ -1205,17 +1227,23 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>155</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
@@ -1231,8 +1259,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>237</v>
+      </c>
       <c r="C4" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H4" s="1">
         <v>15</v>
@@ -1241,24 +1275,27 @@
         <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="H5" s="1">
         <v>45</v>
@@ -1274,17 +1311,20 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>131</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="H6" s="1">
         <v>45</v>
@@ -1300,11 +1340,14 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C7" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="H7" s="1">
         <v>15</v>
@@ -1313,13 +1356,16 @@
         <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K7" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C8" s="1" t="s">
         <v>125</v>
       </c>
@@ -1340,6 +1386,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>82</v>
       </c>
@@ -1360,6 +1409,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1380,11 +1432,14 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H11" s="1">
         <v>1</v>
@@ -1400,26 +1455,32 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C12" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
-      <c r="I12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="K12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C13" s="1" t="s">
         <v>157</v>
       </c>
@@ -1440,6 +1501,9 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>17</v>
       </c>
@@ -1460,6 +1524,9 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1480,6 +1547,9 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
@@ -1499,7 +1569,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1519,7 +1592,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C18" s="1" t="s">
         <v>85</v>
       </c>
@@ -1539,9 +1615,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C19" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>65</v>
@@ -1556,21 +1635,27 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C20" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="I20" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="21" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C21" s="1" t="s">
         <v>160</v>
       </c>
@@ -1590,7 +1675,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>88</v>
       </c>
@@ -1610,7 +1698,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C23" s="1" t="s">
         <v>104</v>
       </c>
@@ -1630,7 +1721,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C24" s="1" t="s">
         <v>3</v>
       </c>
@@ -1650,41 +1744,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C25" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="H25" s="1">
+        <v>2</v>
+      </c>
+      <c r="I25" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H25" s="1">
-        <v>2</v>
-      </c>
-      <c r="I25" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="26" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="H26" s="1">
-        <v>1</v>
-      </c>
-      <c r="I26" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="27" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
       </c>
@@ -1704,7 +1807,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C28" s="1" t="s">
         <v>4</v>
       </c>
@@ -1724,7 +1830,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1744,7 +1853,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C30" s="1" t="s">
         <v>14</v>
       </c>
@@ -1764,12 +1876,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C31" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="H31" s="1">
         <v>2</v>
@@ -1781,7 +1896,10 @@
         <v>115</v>
       </c>
     </row>
-    <row r="32" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C32" s="1" t="s">
         <v>94</v>
       </c>
@@ -1801,7 +1919,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C33" s="1" t="s">
         <v>154</v>
       </c>
@@ -1821,7 +1942,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C34" s="1" t="s">
         <v>29</v>
       </c>
@@ -1841,7 +1965,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C35" s="1" t="s">
         <v>173</v>
       </c>
@@ -1861,7 +1988,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C36" s="1" t="s">
         <v>113</v>
       </c>
@@ -1881,7 +2011,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C37" s="1" t="s">
         <v>8</v>
       </c>
@@ -1901,7 +2034,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C38" s="1" t="s">
         <v>7</v>
       </c>
@@ -1921,9 +2057,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C39" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H39" s="1">
         <v>2</v>
@@ -1935,7 +2074,10 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C40" s="1" t="s">
         <v>5</v>
       </c>
@@ -1955,7 +2097,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C41" s="1" t="s">
         <v>12</v>
       </c>
@@ -1975,12 +2120,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C42" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="H42" s="1">
         <v>3</v>
@@ -1992,7 +2140,10 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C43" s="1" t="s">
         <v>119</v>
       </c>
@@ -2012,7 +2163,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C44" s="1" t="s">
         <v>9</v>
       </c>
@@ -2032,7 +2186,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C45" s="1" t="s">
         <v>33</v>
       </c>
@@ -2052,7 +2209,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C46" s="1" t="s">
         <v>10</v>
       </c>
@@ -2072,7 +2232,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C47" s="1" t="s">
         <v>92</v>
       </c>
@@ -2092,7 +2255,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C48" s="1" t="s">
         <v>124</v>
       </c>
@@ -2112,7 +2278,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C49" s="1" t="s">
         <v>163</v>
       </c>
@@ -2132,7 +2301,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C50" s="1" t="s">
         <v>122</v>
       </c>
@@ -2152,7 +2324,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C51" s="1" t="s">
         <v>83</v>
       </c>
@@ -2172,7 +2347,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C52" s="1" t="s">
         <v>11</v>
       </c>
@@ -2192,7 +2370,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C53" s="3" t="s">
         <v>139</v>
       </c>
@@ -2206,10 +2387,13 @@
         <v>1</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="54" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C54" s="3" t="s">
         <v>107</v>
       </c>
@@ -2223,13 +2407,16 @@
         <v>1</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K54" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C55" s="3" t="s">
         <v>137</v>
       </c>
@@ -2249,7 +2436,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C56" s="1" t="s">
         <v>86</v>
       </c>
@@ -2269,9 +2459,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C57" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D57" s="1">
         <v>600</v>
@@ -2286,7 +2479,10 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C58" s="3" t="s">
         <v>15</v>
       </c>
@@ -2306,7 +2502,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C59" s="3" t="s">
         <v>13</v>
       </c>
@@ -2326,12 +2525,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C60" s="1" t="s">
         <v>100</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H60" s="1">
         <v>2</v>
@@ -2346,7 +2548,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C61" s="1" t="s">
         <v>167</v>
       </c>
@@ -2366,7 +2571,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C62" s="1" t="s">
         <v>36</v>
       </c>
@@ -2386,7 +2594,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C63" s="1" t="s">
         <v>16</v>
       </c>
@@ -2406,7 +2617,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C64" s="1" t="s">
         <v>140</v>
       </c>
@@ -2426,9 +2640,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C65" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>30</v>
@@ -2440,10 +2657,13 @@
         <v>1</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="66" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C66" s="1" t="s">
         <v>21</v>
       </c>
@@ -2463,7 +2683,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C67" s="1" t="s">
         <v>109</v>
       </c>
@@ -2483,7 +2706,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C68" s="1" t="s">
         <v>22</v>
       </c>
@@ -2503,7 +2729,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C69" s="1" t="s">
         <v>23</v>
       </c>
@@ -2523,7 +2752,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C70" s="1" t="s">
         <v>168</v>
       </c>
@@ -2543,9 +2775,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C71" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>142</v>
@@ -2560,9 +2795,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="72" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C72" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>142</v>
@@ -2577,7 +2815,10 @@
         <v>99</v>
       </c>
     </row>
-    <row r="73" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C73" s="3" t="s">
         <v>34</v>
       </c>
@@ -2597,7 +2838,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C74" s="1" t="s">
         <v>111</v>
       </c>
@@ -2617,27 +2861,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C75" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="H75" s="1">
+        <v>2</v>
+      </c>
+      <c r="I75" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J75" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="H75" s="1">
-        <v>2</v>
-      </c>
-      <c r="I75" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J75" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="K75" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C76" s="1" t="s">
         <v>150</v>
       </c>
@@ -2657,7 +2907,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C77" s="3" t="s">
         <v>27</v>
       </c>
@@ -2677,7 +2930,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C78" s="3" t="s">
         <v>31</v>
       </c>
@@ -2697,7 +2953,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C79" s="3" t="s">
         <v>32</v>
       </c>
@@ -2717,9 +2976,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C80" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>78</v>
@@ -2731,9 +2993,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C81" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>78</v>
@@ -2745,7 +3010,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C82" s="1" t="s">
         <v>90</v>
       </c>
@@ -2765,7 +3033,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C83" s="1" t="s">
         <v>24</v>
       </c>
@@ -2785,7 +3056,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C84" s="1" t="s">
         <v>132</v>
       </c>
@@ -2799,7 +3073,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="85" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C85" s="1" t="s">
         <v>127</v>
       </c>
@@ -2807,12 +3084,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C86" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="H86" s="1">
         <v>10</v>
@@ -2821,12 +3101,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C87" s="1" t="s">
         <v>143</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H87" s="1">
         <v>10</v>
@@ -2835,12 +3118,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="3:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C88" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="H88" s="1">
         <v>30</v>
@@ -2849,10 +3135,13 @@
         <v>1</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="89" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C89" s="1" t="s">
         <v>146</v>
       </c>
@@ -2866,7 +3155,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C90" s="1" t="s">
         <v>165</v>
       </c>
@@ -2880,12 +3172,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C91" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="H91" s="1">
         <v>35</v>
@@ -2894,7 +3189,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C92" s="1" t="s">
         <v>110</v>
       </c>
@@ -2908,7 +3206,10 @@
         <v>148</v>
       </c>
     </row>
-    <row r="93" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C93" s="1" t="s">
         <v>128</v>
       </c>
@@ -2922,7 +3223,10 @@
         <v>129</v>
       </c>
     </row>
-    <row r="94" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C94" s="1" t="s">
         <v>171</v>
       </c>
@@ -2936,7 +3240,10 @@
         <v>172</v>
       </c>
     </row>
-    <row r="95" spans="3:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C95" s="1" t="s">
         <v>144</v>
       </c>
@@ -2947,13 +3254,13 @@
         <v>1</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="30" fitToHeight="2" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="51" fitToHeight="2" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Calibri,Regular"&amp;K000000Date_________&amp;C&amp;"Calibri,Regular"&amp;K000000A week deliveries&amp;R&amp;"Calibri,Regular"&amp;U&amp;KFF0000Eggs sold packed on the following dates:</oddHeader>
   </headerFooter>

</xml_diff>